<commit_message>
- BugFix: books which where needed in several terms/curriculums where flagged as "needed" only for students of one term.
</commit_message>
<xml_diff>
--- a/src/main/resources/database/testdata/Buecher_CSG.xlsx
+++ b/src/main/resources/database/testdata/Buecher_CSG.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vorhaben\IntelliJ\OpenSchoolPlatform\src\main\resources\database\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$L$177</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="847">
   <si>
     <t>Jgst</t>
   </si>
@@ -2566,6 +2561,9 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -2885,7 +2883,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2895,24 +2893,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="30.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2950,7 +2948,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -2984,7 +2982,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -3020,7 +3018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -3054,7 +3052,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -3088,7 +3086,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3122,7 +3120,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3156,7 +3154,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -3190,9 +3188,9 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>6</v>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>846</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>57</v>
@@ -3224,7 +3222,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -3258,7 +3256,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -3292,7 +3290,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -3326,7 +3324,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -3362,7 +3360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -3396,7 +3394,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>844</v>
       </c>
@@ -3430,7 +3428,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>6</v>
       </c>
@@ -3466,7 +3464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -3502,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>6</v>
       </c>
@@ -3536,7 +3534,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>6</v>
       </c>
@@ -3570,7 +3568,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -3606,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -3640,7 +3638,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -3674,7 +3672,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -3708,7 +3706,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>6</v>
       </c>
@@ -3742,7 +3740,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>7</v>
       </c>
@@ -3776,7 +3774,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -3812,7 +3810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -3846,7 +3844,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>845</v>
       </c>
@@ -3880,7 +3878,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>7</v>
       </c>
@@ -3914,7 +3912,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>7</v>
       </c>
@@ -3950,7 +3948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>7</v>
       </c>
@@ -3986,7 +3984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>7</v>
       </c>
@@ -4020,7 +4018,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>7</v>
       </c>
@@ -4054,7 +4052,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>7</v>
       </c>
@@ -4090,7 +4088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>7</v>
       </c>
@@ -4124,7 +4122,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>7</v>
       </c>
@@ -4158,7 +4156,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>7</v>
       </c>
@@ -4192,7 +4190,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>7</v>
       </c>
@@ -4226,7 +4224,7 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>8</v>
       </c>
@@ -4260,7 +4258,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>8</v>
       </c>
@@ -4296,7 +4294,7 @@
       </c>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>8</v>
       </c>
@@ -4330,7 +4328,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -4366,7 +4364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>8</v>
       </c>
@@ -4402,7 +4400,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>8</v>
       </c>
@@ -4436,7 +4434,7 @@
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>8</v>
       </c>
@@ -4470,7 +4468,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>8</v>
       </c>
@@ -4504,7 +4502,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>8</v>
       </c>
@@ -4540,7 +4538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>8</v>
       </c>
@@ -4576,7 +4574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>8</v>
       </c>
@@ -4614,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>8</v>
       </c>
@@ -4652,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>8</v>
       </c>
@@ -4686,7 +4684,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>8</v>
       </c>
@@ -4720,7 +4718,7 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>8</v>
       </c>
@@ -4756,7 +4754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>8</v>
       </c>
@@ -4790,7 +4788,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>8</v>
       </c>
@@ -4824,7 +4822,7 @@
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>8</v>
       </c>
@@ -4858,7 +4856,7 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>8</v>
       </c>
@@ -4896,7 +4894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>8</v>
       </c>
@@ -4934,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>9</v>
       </c>
@@ -4968,7 +4966,7 @@
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>9</v>
       </c>
@@ -5004,7 +5002,7 @@
       </c>
       <c r="L60" s="1"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>9</v>
       </c>
@@ -5040,7 +5038,7 @@
       </c>
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>9</v>
       </c>
@@ -5074,7 +5072,7 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>9</v>
       </c>
@@ -5110,7 +5108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>9</v>
       </c>
@@ -5144,7 +5142,7 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>9</v>
       </c>
@@ -5178,7 +5176,7 @@
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>9</v>
       </c>
@@ -5214,7 +5212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>9</v>
       </c>
@@ -5250,7 +5248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>9</v>
       </c>
@@ -5288,7 +5286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>9</v>
       </c>
@@ -5326,7 +5324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>9</v>
       </c>
@@ -5360,7 +5358,7 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>9</v>
       </c>
@@ -5394,7 +5392,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>9</v>
       </c>
@@ -5428,7 +5426,7 @@
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>9</v>
       </c>
@@ -5462,7 +5460,7 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>9</v>
       </c>
@@ -5498,7 +5496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>9</v>
       </c>
@@ -5534,7 +5532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>9</v>
       </c>
@@ -5568,7 +5566,7 @@
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>9</v>
       </c>
@@ -5602,7 +5600,7 @@
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>9</v>
       </c>
@@ -5636,7 +5634,7 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>9</v>
       </c>
@@ -5674,7 +5672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>8</v>
       </c>
@@ -5712,7 +5710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>9</v>
       </c>
@@ -5746,7 +5744,7 @@
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>10</v>
       </c>
@@ -5780,7 +5778,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>10</v>
       </c>
@@ -5816,7 +5814,7 @@
       </c>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>10</v>
       </c>
@@ -5852,7 +5850,7 @@
       </c>
       <c r="L84" s="1"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>10</v>
       </c>
@@ -5886,7 +5884,7 @@
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>10</v>
       </c>
@@ -5922,7 +5920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>10</v>
       </c>
@@ -5956,7 +5954,7 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>10</v>
       </c>
@@ -5990,7 +5988,7 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>10</v>
       </c>
@@ -6024,7 +6022,7 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>10</v>
       </c>
@@ -6060,7 +6058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>10</v>
       </c>
@@ -6096,7 +6094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>10</v>
       </c>
@@ -6134,7 +6132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>10</v>
       </c>
@@ -6172,7 +6170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>10</v>
       </c>
@@ -6206,7 +6204,7 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>10</v>
       </c>
@@ -6240,7 +6238,7 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>10</v>
       </c>
@@ -6274,7 +6272,7 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>10</v>
       </c>
@@ -6310,7 +6308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>10</v>
       </c>
@@ -6346,7 +6344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>10</v>
       </c>
@@ -6380,7 +6378,7 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>10</v>
       </c>
@@ -6414,7 +6412,7 @@
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>10</v>
       </c>
@@ -6448,7 +6446,7 @@
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>10</v>
       </c>
@@ -6486,7 +6484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>10</v>
       </c>
@@ -6524,7 +6522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>10</v>
       </c>
@@ -6558,7 +6556,7 @@
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>10</v>
       </c>
@@ -6594,7 +6592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>10</v>
       </c>
@@ -6628,7 +6626,7 @@
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>11</v>
       </c>
@@ -6662,7 +6660,7 @@
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>11</v>
       </c>
@@ -6696,7 +6694,7 @@
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>11</v>
       </c>
@@ -6730,7 +6728,7 @@
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>11</v>
       </c>
@@ -6764,7 +6762,7 @@
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>11</v>
       </c>
@@ -6798,7 +6796,7 @@
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>11</v>
       </c>
@@ -6834,7 +6832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>11</v>
       </c>
@@ -6868,7 +6866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>11</v>
       </c>
@@ -6904,7 +6902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>11</v>
       </c>
@@ -6940,7 +6938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>11</v>
       </c>
@@ -6972,7 +6970,7 @@
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>11</v>
       </c>
@@ -7006,7 +7004,7 @@
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>11</v>
       </c>
@@ -7040,7 +7038,7 @@
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>11</v>
       </c>
@@ -7074,7 +7072,7 @@
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>11</v>
       </c>
@@ -7108,7 +7106,7 @@
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>11</v>
       </c>
@@ -7144,7 +7142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>11</v>
       </c>
@@ -7180,7 +7178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>11</v>
       </c>
@@ -7216,7 +7214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>11</v>
       </c>
@@ -7250,7 +7248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>11</v>
       </c>
@@ -7282,7 +7280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>11</v>
       </c>
@@ -7314,7 +7312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>11</v>
       </c>
@@ -7348,7 +7346,7 @@
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>11</v>
       </c>
@@ -7382,7 +7380,7 @@
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>11</v>
       </c>
@@ -7416,7 +7414,7 @@
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>11</v>
       </c>
@@ -7450,7 +7448,7 @@
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>11</v>
       </c>
@@ -7484,7 +7482,7 @@
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>11</v>
       </c>
@@ -7518,7 +7516,7 @@
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>11</v>
       </c>
@@ -7550,7 +7548,7 @@
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>11</v>
       </c>
@@ -7584,7 +7582,7 @@
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>11</v>
       </c>
@@ -7618,7 +7616,7 @@
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>11</v>
       </c>
@@ -7652,7 +7650,7 @@
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>11</v>
       </c>
@@ -7686,7 +7684,7 @@
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>11</v>
       </c>
@@ -7720,7 +7718,7 @@
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>11</v>
       </c>
@@ -7754,7 +7752,7 @@
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>11</v>
       </c>
@@ -7790,7 +7788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>11</v>
       </c>
@@ -7826,7 +7824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>11</v>
       </c>
@@ -7862,7 +7860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>11</v>
       </c>
@@ -7896,7 +7894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>11</v>
       </c>
@@ -7930,7 +7928,7 @@
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>11</v>
       </c>
@@ -7966,7 +7964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>11</v>
       </c>
@@ -8000,7 +7998,7 @@
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>11</v>
       </c>
@@ -8034,7 +8032,7 @@
       <c r="K147" s="1"/>
       <c r="L147" s="1"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>11</v>
       </c>
@@ -8068,7 +8066,7 @@
       <c r="K148" s="1"/>
       <c r="L148" s="1"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>12</v>
       </c>
@@ -8102,7 +8100,7 @@
       <c r="K149" s="1"/>
       <c r="L149" s="1"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>11</v>
       </c>
@@ -8136,7 +8134,7 @@
       <c r="K150" s="1"/>
       <c r="L150" s="1"/>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>11</v>
       </c>
@@ -8170,7 +8168,7 @@
       <c r="K151" s="1"/>
       <c r="L151" s="1"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>11</v>
       </c>
@@ -8204,7 +8202,7 @@
       <c r="K152" s="1"/>
       <c r="L152" s="1"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>11</v>
       </c>
@@ -8238,7 +8236,7 @@
       <c r="K153" s="1"/>
       <c r="L153" s="1"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>12</v>
       </c>
@@ -8272,7 +8270,7 @@
       <c r="K154" s="1"/>
       <c r="L154" s="1"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>12</v>
       </c>
@@ -8306,7 +8304,7 @@
       <c r="K155" s="1"/>
       <c r="L155" s="1"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>12</v>
       </c>
@@ -8340,7 +8338,7 @@
       <c r="K156" s="1"/>
       <c r="L156" s="1"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>12</v>
       </c>
@@ -8376,7 +8374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>12</v>
       </c>
@@ -8410,7 +8408,7 @@
       <c r="K158" s="1"/>
       <c r="L158" s="1"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>12</v>
       </c>
@@ -8444,7 +8442,7 @@
       <c r="K159" s="1"/>
       <c r="L159" s="1"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>12</v>
       </c>
@@ -8478,7 +8476,7 @@
       <c r="K160" s="1"/>
       <c r="L160" s="1"/>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>12</v>
       </c>
@@ -8512,7 +8510,7 @@
       <c r="K161" s="1"/>
       <c r="L161" s="1"/>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>12</v>
       </c>
@@ -8546,7 +8544,7 @@
       <c r="K162" s="1"/>
       <c r="L162" s="1"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>12</v>
       </c>
@@ -8582,7 +8580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>12</v>
       </c>
@@ -8618,7 +8616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>12</v>
       </c>
@@ -8654,7 +8652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>12</v>
       </c>
@@ -8688,7 +8686,7 @@
       <c r="K166" s="1"/>
       <c r="L166" s="1"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>12</v>
       </c>
@@ -8722,7 +8720,7 @@
       <c r="K167" s="1"/>
       <c r="L167" s="1"/>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>12</v>
       </c>
@@ -8756,7 +8754,7 @@
       <c r="K168" s="1"/>
       <c r="L168" s="1"/>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>12</v>
       </c>
@@ -8792,7 +8790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>12</v>
       </c>
@@ -8828,7 +8826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>12</v>
       </c>
@@ -8864,7 +8862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>12</v>
       </c>
@@ -8900,7 +8898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>12</v>
       </c>
@@ -8934,7 +8932,7 @@
       <c r="K173" s="1"/>
       <c r="L173" s="1"/>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>12</v>
       </c>
@@ -8968,7 +8966,7 @@
       <c r="K174" s="1"/>
       <c r="L174" s="1"/>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>12</v>
       </c>
@@ -9002,7 +9000,7 @@
       <c r="K175" s="1"/>
       <c r="L175" s="1"/>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>12</v>
       </c>
@@ -9036,7 +9034,7 @@
       <c r="K176" s="1"/>
       <c r="L176" s="1"/>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>12</v>
       </c>
@@ -9083,7 +9081,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>